<commit_message>
make all additional stores yellow
</commit_message>
<xml_diff>
--- a/07-21-24 to 07-27-24 Milwaukee Schedule Copy.xlsx
+++ b/07-21-24 to 07-27-24 Milwaukee Schedule Copy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y80"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>Makeda</t>
+          <t>Qiana</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>Qiana</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="W35" t="inlineStr">
@@ -2754,21 +2754,9 @@
         </is>
       </c>
       <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>23)</t>
-        </is>
-      </c>
-      <c r="V36" t="inlineStr">
-        <is>
-          <t>Taylor</t>
-        </is>
-      </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>@ Store</t>
-        </is>
-      </c>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
     </row>
@@ -2849,7 +2837,11 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>5:00 AM MEET OFFICE</t>
+        </is>
+      </c>
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
@@ -2895,7 +2887,7 @@
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr">
         <is>
-          <t>5:00 AM MEET OFFICE</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W39" t="inlineStr"/>
@@ -2907,22 +2899,9 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>2)</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Carlie</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Trevor)</t>
-        </is>
-      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
@@ -2951,7 +2930,7 @@
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W40" t="inlineStr"/>
@@ -2965,15 +2944,20 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Jerry D</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr"/>
+          <t>Carlie</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>@ Store
+(w/ Trevor)</t>
+        </is>
+      </c>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
@@ -2984,25 +2968,17 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>DC5-FINANCIAL</t>
-        </is>
-      </c>
+      <c r="R41" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>ROTE OIL #14 TREVOR (CITGO)</t>
         </is>
       </c>
       <c r="W41" t="inlineStr"/>
@@ -3016,12 +2992,12 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Jerry D</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -3037,7 +3013,7 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
-          <t>ROTE OIL #10 MUKWONAGO - ROCHESTER</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="O42" t="inlineStr"/>
@@ -3045,7 +3021,7 @@
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr">
         <is>
-          <t>ROTE OIL #1 PADDOCK LAKE- BRASS BALL</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="S42" t="inlineStr"/>
@@ -3053,7 +3029,7 @@
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr">
         <is>
-          <t>ROTE OIL #14 TREVOR (CITGO)</t>
+          <t>12617 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W42" t="inlineStr"/>
@@ -3067,12 +3043,12 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Sue</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -3088,7 +3064,7 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr">
         <is>
-          <t>1060 N ROCHESTER ST</t>
+          <t>ROTE OIL #10 MUKWONAGO - ROCHESTER</t>
         </is>
       </c>
       <c r="O43" t="inlineStr"/>
@@ -3096,7 +3072,7 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr">
         <is>
-          <t>25406 75TH ST</t>
+          <t>ROTE OIL #1 PADDOCK LAKE- BRASS BALL</t>
         </is>
       </c>
       <c r="S43" t="inlineStr"/>
@@ -3104,7 +3080,7 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr">
         <is>
-          <t>12617 ANTIOCH RD</t>
+          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
         </is>
       </c>
       <c r="W43" t="inlineStr"/>
@@ -3118,20 +3094,15 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>6)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Trevor</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Carlie)</t>
-        </is>
-      </c>
+          <t>Sue</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
@@ -3144,7 +3115,7 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/dmvR5bTHLs1Cbjcr5</t>
+          <t>1060 N ROCHESTER ST</t>
         </is>
       </c>
       <c r="O44" t="inlineStr"/>
@@ -3152,7 +3123,7 @@
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/LTa4ckcczx5qc8269</t>
+          <t>25406 75TH ST</t>
         </is>
       </c>
       <c r="S44" t="inlineStr"/>
@@ -3160,7 +3131,7 @@
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="W44" t="inlineStr"/>
@@ -3172,9 +3143,22 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>6)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Trevor</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>@ Store
+(w/ Carlie)</t>
+        </is>
+      </c>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
@@ -3187,7 +3171,7 @@
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>https://goo.gl/maps/dmvR5bTHLs1Cbjcr5</t>
         </is>
       </c>
       <c r="O45" t="inlineStr"/>
@@ -3195,7 +3179,7 @@
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>https://goo.gl/maps/LTa4ckcczx5qc8269</t>
         </is>
       </c>
       <c r="S45" t="inlineStr"/>
@@ -3203,7 +3187,7 @@
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W45" t="inlineStr"/>
@@ -3230,7 +3214,7 @@
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="O46" t="inlineStr"/>
@@ -3238,7 +3222,7 @@
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="S46" t="inlineStr"/>
@@ -3246,7 +3230,7 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>ROTE OIL #13 TREVOR (BP)</t>
         </is>
       </c>
       <c r="W46" t="inlineStr"/>
@@ -3258,16 +3242,8 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>5:00 AM OFFICE LEAVE TIME</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr"/>
@@ -3281,7 +3257,7 @@
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr">
         <is>
-          <t>ROTE OIL #12 MUKWONAGO - (AMOCO) GREENWALD</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -3289,7 +3265,7 @@
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr">
         <is>
-          <t>ROTE OIL #2 PADDOCK LAKE- 75TH ST</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="S47" t="inlineStr"/>
@@ -3297,7 +3273,7 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>ROTE OIL #13 TREVOR (BP)</t>
+          <t>12511 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
@@ -3316,7 +3292,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve">6:00 AM START </t>
+          <t>5:00 AM OFFICE LEAVE TIME</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -3332,7 +3308,7 @@
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr">
         <is>
-          <t>909 GREENWALD CT</t>
+          <t>ROTE OIL #12 MUKWONAGO - (AMOCO) GREENWALD</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -3340,7 +3316,7 @@
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
         <is>
-          <t>25555 75TH ST</t>
+          <t>ROTE OIL #2 PADDOCK LAKE- 75TH ST</t>
         </is>
       </c>
       <c r="S48" t="inlineStr"/>
@@ -3348,7 +3324,7 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>12511 ANTIOCH RD</t>
+          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
@@ -3360,10 +3336,14 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve">DC5-FINANCIAL </t>
+          <t xml:space="preserve">6:00 AM START </t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -3379,7 +3359,7 @@
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/ejQSLoz2D8EmzKVq6</t>
+          <t>909 GREENWALD CT</t>
         </is>
       </c>
       <c r="O49" t="inlineStr"/>
@@ -3387,17 +3367,13 @@
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/5UyWWXXbzXMaVnv99</t>
+          <t>25555 75TH ST</t>
         </is>
       </c>
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
-        </is>
-      </c>
+      <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
@@ -3410,7 +3386,7 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>ROTE OIL #03 TWIN LAKES</t>
+          <t xml:space="preserve">DC5-FINANCIAL </t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3426,18 +3402,34 @@
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>https://goo.gl/maps/ejQSLoz2D8EmzKVq6</t>
         </is>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/5UyWWXXbzXMaVnv99</t>
+        </is>
+      </c>
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
-      <c r="V50" t="inlineStr"/>
-      <c r="W50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>Equip</t>
+        </is>
+      </c>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
     </row>
@@ -3449,7 +3441,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>475 N LAKE AVE</t>
+          <t>ROTE OIL #03 TWIN LAKES</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3465,40 +3457,29 @@
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve">DC5-FINANCIAL </t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>Brianna</t>
-        </is>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Ian</t>
         </is>
       </c>
       <c r="W51" t="inlineStr">
         <is>
-          <t>Equip</t>
+          <t>Driver,
+Optima</t>
         </is>
       </c>
       <c r="X51" t="inlineStr"/>
@@ -3512,7 +3493,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://goo.gl/maps/jNgJR8hii6jJGZQP7 </t>
+          <t>475 N LAKE AVE</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3528,43 +3509,38 @@
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr">
         <is>
-          <t>ROTE OIL  #11 MUKWONAGO - (BP) ARROWHEAD</t>
+          <t xml:space="preserve">DC5-FINANCIAL </t>
         </is>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Brianna</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
         <is>
-          <t>Optima</t>
+          <t>@ Store, Equip</t>
         </is>
       </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>Ian</t>
-        </is>
-      </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>Driver,
-Optima</t>
-        </is>
-      </c>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr"/>
       <c r="Y52" t="inlineStr"/>
     </row>
@@ -3576,7 +3552,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t xml:space="preserve">https://goo.gl/maps/jNgJR8hii6jJGZQP7 </t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3592,14 +3568,26 @@
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr">
         <is>
-          <t>122 ARROWHEAD DR</t>
+          <t>ROTE OIL  #11 MUKWONAGO - (BP) ARROWHEAD</t>
         </is>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>Optima</t>
+        </is>
+      </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
@@ -3615,7 +3603,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3631,7 +3619,7 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/7XkTFZtDFDgGBctz7</t>
+          <t>122 ARROWHEAD DR</t>
         </is>
       </c>
       <c r="O54" t="inlineStr"/>
@@ -3641,7 +3629,11 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr"/>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>5:30 AM MEET BAYSHORE</t>
+        </is>
+      </c>
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
@@ -3654,7 +3646,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>ROTE OIL #04 GENOA CITY</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3668,21 +3660,21 @@
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/7XkTFZtDFDgGBctz7</t>
+        </is>
+      </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="R55" t="inlineStr"/>
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr">
         <is>
-          <t>5:30 AM MEET BAYSHORE</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="W55" t="inlineStr"/>
@@ -3697,7 +3689,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t xml:space="preserve">100 ELIZABETH LANE    </t>
+          <t>ROTE OIL #04 GENOA CITY</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3710,26 +3702,14 @@
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>Brianna</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="S56" t="inlineStr"/>
@@ -3737,7 +3717,7 @@
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="W56" t="inlineStr"/>
@@ -3752,7 +3732,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/DitGJzEvTVhJPxkJ8</t>
+          <t xml:space="preserve">100 ELIZABETH LANE    </t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3767,20 +3747,24 @@
       <c r="L57" t="inlineStr"/>
       <c r="M57" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>Ian</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr"/>
+          <t>Brianna</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>@ Store, Equip</t>
+        </is>
+      </c>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr">
         <is>
-          <t>AURORA OUTPATIENT RX #1760, OAK CREEK</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="S57" t="inlineStr"/>
@@ -3788,7 +3772,7 @@
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>AURORA OUTPATIENT RX #1155 DEPERE</t>
         </is>
       </c>
       <c r="W57" t="inlineStr"/>
@@ -3803,7 +3787,7 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t xml:space="preserve">TO FOLLOW   </t>
+          <t>https://goo.gl/maps/DitGJzEvTVhJPxkJ8</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3816,14 +3800,22 @@
       </c>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>Ian</t>
+        </is>
+      </c>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr">
         <is>
-          <t>200 E RYAN ROAD, SUITE 101</t>
+          <t>AURORA OUTPATIENT RX #1760, OAK CREEK</t>
         </is>
       </c>
       <c r="S58" t="inlineStr"/>
@@ -3831,7 +3823,7 @@
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr">
         <is>
-          <t>AURORA OUTPATIENT RX #1155 DEPERE</t>
+          <t>1881 CHICAGO ST</t>
         </is>
       </c>
       <c r="W58" t="inlineStr"/>
@@ -3846,7 +3838,7 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t xml:space="preserve">TO FOLLOW   </t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3866,7 +3858,7 @@
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/5XiBYxoT2sF2</t>
+          <t>200 E RYAN ROAD, SUITE 101</t>
         </is>
       </c>
       <c r="S59" t="inlineStr"/>
@@ -3874,7 +3866,7 @@
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr">
         <is>
-          <t>1881 CHICAGO ST</t>
+          <t>https://goo.gl/maps/9vepkQciLjQDFTRi8</t>
         </is>
       </c>
       <c r="W59" t="inlineStr"/>
@@ -3889,7 +3881,7 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>ROTE OIL #05  LAKE GENEVA</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3899,23 +3891,19 @@
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
       <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>6:00 AM START</t>
-        </is>
-      </c>
+      <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
-      <c r="R60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/5XiBYxoT2sF2</t>
+        </is>
+      </c>
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
-      <c r="V60" t="inlineStr">
-        <is>
-          <t>https://goo.gl/maps/9vepkQciLjQDFTRi8</t>
-        </is>
-      </c>
+      <c r="V60" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>
       <c r="Y60" t="inlineStr"/>
@@ -3928,7 +3916,7 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>300 PELLER RD</t>
+          <t>ROTE OIL #05  LAKE GENEVA</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -3952,30 +3940,31 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr">
         <is>
-          <t xml:space="preserve">DC5-ITEM LEVEL </t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr">
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr">
         <is>
           <t>1)</t>
         </is>
       </c>
-      <c r="R61" t="inlineStr">
+      <c r="V61" t="inlineStr">
         <is>
           <t>DJ</t>
         </is>
       </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>Equip</t>
-        </is>
-      </c>
-      <c r="T61" t="inlineStr"/>
-      <c r="U61" t="inlineStr"/>
-      <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr"/>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>Driver,
+Altima, Equip</t>
+        </is>
+      </c>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
     </row>
@@ -3987,7 +3976,7 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/6fegzT1PbyY5VkDR6</t>
+          <t>300 PELLER RD</t>
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
@@ -4007,29 +3996,40 @@
       <c r="M62" t="inlineStr"/>
       <c r="N62" t="inlineStr">
         <is>
-          <t>AURORA OUTPATIENT RX #1135 OCONOMOWOC</t>
+          <t xml:space="preserve">DC5-ITEM LEVEL </t>
         </is>
       </c>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="inlineStr"/>
-      <c r="R62" t="inlineStr"/>
-      <c r="S62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>1)</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>DJ</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>Equip</t>
+        </is>
+      </c>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr">
         <is>
-          <t>1)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>DJ</t>
+          <t>Casey</t>
         </is>
       </c>
       <c r="W62" t="inlineStr">
         <is>
-          <t>Driver,
-Altima, Equip</t>
+          <t>3rd Aurora</t>
         </is>
       </c>
       <c r="X62" t="inlineStr"/>
@@ -4041,7 +4041,11 @@
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/6fegzT1PbyY5VkDR6</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
@@ -4059,7 +4063,7 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr">
         <is>
-          <t>1284 SUMMIT AVENUE SUITE 100</t>
+          <t>AURORA OUTPATIENT RX #1135 OCONOMOWOC</t>
         </is>
       </c>
       <c r="O63" t="inlineStr"/>
@@ -4070,19 +4074,15 @@
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>Casey</t>
-        </is>
-      </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>3rd Aurora</t>
-        </is>
-      </c>
+          <t>Lashaun</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr"/>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
     </row>
@@ -4091,21 +4091,9 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Brianna</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>@ Store, Equip</t>
-        </is>
-      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
@@ -4114,17 +4102,13 @@
       <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/wL6wpeCnhYBhsPmP7</t>
+          <t>1284 SUMMIT AVENUE SUITE 100</t>
         </is>
       </c>
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>Office</t>
-        </is>
-      </c>
+      <c r="R64" t="inlineStr"/>
       <c r="S64" t="inlineStr"/>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
@@ -4140,17 +4124,17 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>Brianna</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Gold Camry</t>
+          <t>@ Store, Equip</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -4159,13 +4143,17 @@
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
-      <c r="N65" t="inlineStr"/>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/wL6wpeCnhYBhsPmP7</t>
+        </is>
+      </c>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Office</t>
         </is>
       </c>
       <c r="S65" t="inlineStr"/>
@@ -4181,9 +4169,21 @@
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Katherine</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Gold Camry</t>
+        </is>
+      </c>
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
@@ -4193,24 +4193,16 @@
       </c>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>Kim</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Sante Fe available, Equip</t>
-        </is>
-      </c>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>
-      <c r="R66" t="inlineStr"/>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Lashaun</t>
+        </is>
+      </c>
       <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
@@ -4238,15 +4230,19 @@
       <c r="L67" t="inlineStr"/>
       <c r="M67" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>Cynthia</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr"/>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Sante Fe available, Equip</t>
+        </is>
+      </c>
       <c r="P67" t="inlineStr"/>
       <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr"/>
@@ -4275,8 +4271,16 @@
       </c>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>Cynthia</t>
+        </is>
+      </c>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
       <c r="Q68" t="inlineStr"/>
@@ -4338,11 +4342,7 @@
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
       <c r="M70" t="inlineStr"/>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>6:30 AM MEET COLLEGE (SOUTHWEST)</t>
-        </is>
-      </c>
+      <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
@@ -4371,7 +4371,7 @@
       <c r="M71" t="inlineStr"/>
       <c r="N71" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>6:30 AM MEET COLLEGE (SOUTHWEST)</t>
         </is>
       </c>
       <c r="O71" t="inlineStr"/>
@@ -4414,7 +4414,7 @@
       <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr">
         <is>
-          <t xml:space="preserve">DC5-ITEM LEVEL  </t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="O72" t="inlineStr"/>
@@ -4445,7 +4445,7 @@
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr">
         <is>
-          <t>OPEN PANTRY #493, RACINE</t>
+          <t xml:space="preserve">DC5-ITEM LEVEL  </t>
         </is>
       </c>
       <c r="O73" t="inlineStr"/>
@@ -4476,7 +4476,7 @@
       <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr">
         <is>
-          <t>3441 SPRING ST</t>
+          <t>OPEN PANTRY #493, RACINE</t>
         </is>
       </c>
       <c r="O74" t="inlineStr"/>
@@ -4511,7 +4511,7 @@
       <c r="M75" t="inlineStr"/>
       <c r="N75" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/8i7XHemjTpL2</t>
+          <t>3441 SPRING ST</t>
         </is>
       </c>
       <c r="O75" t="inlineStr"/>
@@ -4544,7 +4544,11 @@
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
       <c r="M76" t="inlineStr"/>
-      <c r="N76" t="inlineStr"/>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/8i7XHemjTpL2</t>
+        </is>
+      </c>
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="inlineStr"/>
@@ -4570,21 +4574,9 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>Katherine</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>Equip</t>
-        </is>
-      </c>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>
@@ -4611,18 +4603,17 @@
       <c r="L78" t="inlineStr"/>
       <c r="M78" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Driver,
-Red Van</t>
+          <t>Equip</t>
         </is>
       </c>
       <c r="P78" t="inlineStr"/>
@@ -4651,15 +4642,20 @@
       <c r="L79" t="inlineStr"/>
       <c r="M79" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr"/>
+          <t>Casey</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Driver,
+Red Van</t>
+        </is>
+      </c>
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr"/>
@@ -4686,12 +4682,12 @@
       <c r="L80" t="inlineStr"/>
       <c r="M80" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="O80" t="inlineStr"/>
@@ -4706,6 +4702,41 @@
       <c r="X80" t="inlineStr"/>
       <c r="Y80" t="inlineStr"/>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>4)</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
+      <c r="R81" t="inlineStr"/>
+      <c r="S81" t="inlineStr"/>
+      <c r="T81" t="inlineStr"/>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
prep for grafton team
</commit_message>
<xml_diff>
--- a/07-21-24 to 07-27-24 Milwaukee Schedule Copy.xlsx
+++ b/07-21-24 to 07-27-24 Milwaukee Schedule Copy.xlsx
@@ -2837,11 +2837,7 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr">
-        <is>
-          <t>5:00 AM MEET OFFICE</t>
-        </is>
-      </c>
+      <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
@@ -2877,17 +2873,13 @@
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>5:00 AM OFFICE LEAVE TIME</t>
-        </is>
-      </c>
+      <c r="R39" t="inlineStr"/>
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>5:00 AM MEET OFFICE</t>
         </is>
       </c>
       <c r="W39" t="inlineStr"/>
@@ -2899,9 +2891,22 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Carlie</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>@ Store
+(w/ Trevor)</t>
+        </is>
+      </c>
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
@@ -2912,17 +2917,13 @@
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">5:30 AM START </t>
-        </is>
-      </c>
+      <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr">
         <is>
-          <t>6:00 AM START</t>
+          <t>5:00 AM OFFICE LEAVE TIME</t>
         </is>
       </c>
       <c r="S40" t="inlineStr"/>
@@ -2930,7 +2931,7 @@
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>6:00 AM START</t>
         </is>
       </c>
       <c r="W40" t="inlineStr"/>
@@ -2944,20 +2945,15 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>3)</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Carlie</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Trevor)</t>
-        </is>
-      </c>
+          <t>Jerry D</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
@@ -2968,17 +2964,25 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5:30 AM START </t>
+        </is>
+      </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>6:00 AM START</t>
+        </is>
+      </c>
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr">
         <is>
-          <t>ROTE OIL #14 TREVOR (CITGO)</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W41" t="inlineStr"/>
@@ -2992,12 +2996,12 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>4)</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Jerry D</t>
+          <t>Lashaun</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -3029,7 +3033,7 @@
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr">
         <is>
-          <t>12617 ANTIOCH RD</t>
+          <t>ROTE OIL #14 TREVOR (CITGO)</t>
         </is>
       </c>
       <c r="W42" t="inlineStr"/>
@@ -3043,12 +3047,12 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4)</t>
+          <t>5)</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Lashaun</t>
+          <t>Sue</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -3080,7 +3084,7 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
+          <t>12617 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W43" t="inlineStr"/>
@@ -3094,15 +3098,20 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>5)</t>
+          <t>6)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Sue</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
+          <t>Trevor</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>@ Store
+(w/ Carlie)</t>
+        </is>
+      </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
@@ -3131,7 +3140,7 @@
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr">
         <is>
-          <t>TO FOLLOW</t>
+          <t>https://goo.gl/maps/xA9YMzPGc6Vhxi5r8</t>
         </is>
       </c>
       <c r="W44" t="inlineStr"/>
@@ -3143,22 +3152,9 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>6)</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Trevor</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>@ Store
-(w/ Carlie)</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
@@ -3187,7 +3183,7 @@
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr">
         <is>
-          <t>DC5-FINANCIAL</t>
+          <t>TO FOLLOW</t>
         </is>
       </c>
       <c r="W45" t="inlineStr"/>
@@ -3230,7 +3226,7 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr">
         <is>
-          <t>ROTE OIL #13 TREVOR (BP)</t>
+          <t>DC5-FINANCIAL</t>
         </is>
       </c>
       <c r="W46" t="inlineStr"/>
@@ -3273,7 +3269,7 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>12511 ANTIOCH RD</t>
+          <t>ROTE OIL #13 TREVOR (BP)</t>
         </is>
       </c>
       <c r="W47" t="inlineStr"/>
@@ -3324,7 +3320,7 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
+          <t>12511 ANTIOCH RD</t>
         </is>
       </c>
       <c r="W48" t="inlineStr"/>
@@ -3373,7 +3369,11 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr"/>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/iu3xzNwgJ32esP5RA</t>
+        </is>
+      </c>
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
@@ -3415,21 +3415,9 @@
       </c>
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>Katherine</t>
-        </is>
-      </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>Equip</t>
-        </is>
-      </c>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
     </row>
@@ -3468,18 +3456,17 @@
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>Ian</t>
+          <t>Katherine</t>
         </is>
       </c>
       <c r="W51" t="inlineStr">
         <is>
-          <t>Driver,
-Optima</t>
+          <t>Equip</t>
         </is>
       </c>
       <c r="X51" t="inlineStr"/>
@@ -3532,15 +3519,20 @@
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
-      <c r="W52" t="inlineStr"/>
+          <t>Ian</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>Driver,
+Optima</t>
+        </is>
+      </c>
       <c r="X52" t="inlineStr"/>
       <c r="Y52" t="inlineStr"/>
     </row>
@@ -3629,11 +3621,7 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
-      <c r="V54" t="inlineStr">
-        <is>
-          <t>5:30 AM MEET BAYSHORE</t>
-        </is>
-      </c>
+      <c r="V54" t="inlineStr"/>
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
@@ -3674,7 +3662,7 @@
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr">
         <is>
-          <t>7:00 AM START</t>
+          <t>5:30 AM MEET BAYSHORE</t>
         </is>
       </c>
       <c r="W55" t="inlineStr"/>
@@ -3717,7 +3705,7 @@
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr">
         <is>
-          <t>DC5-ITEM LEVEL</t>
+          <t>7:00 AM START</t>
         </is>
       </c>
       <c r="W56" t="inlineStr"/>
@@ -3772,7 +3760,7 @@
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr">
         <is>
-          <t>AURORA OUTPATIENT RX #1155 DEPERE</t>
+          <t>DC5-ITEM LEVEL</t>
         </is>
       </c>
       <c r="W57" t="inlineStr"/>
@@ -3823,7 +3811,7 @@
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr">
         <is>
-          <t>1881 CHICAGO ST</t>
+          <t>AURORA OUTPATIENT RX #1155 DEPERE</t>
         </is>
       </c>
       <c r="W58" t="inlineStr"/>
@@ -3866,7 +3854,7 @@
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://goo.gl/maps/9vepkQciLjQDFTRi8</t>
+          <t>1881 CHICAGO ST</t>
         </is>
       </c>
       <c r="W59" t="inlineStr"/>
@@ -3903,7 +3891,11 @@
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
-      <c r="V60" t="inlineStr"/>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>https://goo.gl/maps/9vepkQciLjQDFTRi8</t>
+        </is>
+      </c>
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>
       <c r="Y60" t="inlineStr"/>
@@ -3949,22 +3941,9 @@
       <c r="R61" t="inlineStr"/>
       <c r="S61" t="inlineStr"/>
       <c r="T61" t="inlineStr"/>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>1)</t>
-        </is>
-      </c>
-      <c r="V61" t="inlineStr">
-        <is>
-          <t>DJ</t>
-        </is>
-      </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>Driver,
-Altima, Equip</t>
-        </is>
-      </c>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
     </row>
@@ -4019,17 +3998,18 @@
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr">
         <is>
-          <t>2)</t>
+          <t>1)</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>Casey</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="W62" t="inlineStr">
         <is>
-          <t>3rd Aurora</t>
+          <t>Driver,
+Altima, Equip</t>
         </is>
       </c>
       <c r="X62" t="inlineStr"/>
@@ -4074,15 +4054,19 @@
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr">
         <is>
-          <t>3)</t>
+          <t>2)</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>Lashaun</t>
-        </is>
-      </c>
-      <c r="W63" t="inlineStr"/>
+          <t>Casey</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>3rd Aurora</t>
+        </is>
+      </c>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
     </row>

</xml_diff>